<commit_message>
Work on PRS / disease relationship
</commit_message>
<xml_diff>
--- a/0_DATA/list_of_traits_GSMR.xlsx
+++ b/0_DATA/list_of_traits_GSMR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38160" yWindow="620" windowWidth="37780" windowHeight="20400" tabRatio="500"/>
+    <workbookView xWindow="-38160" yWindow="460" windowWidth="37780" windowHeight="19480" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="224">
   <si>
     <t>Trait</t>
   </si>
@@ -967,6 +967,12 @@
   <si>
     <t>3 fichiers. A chosiir. + stat a faire pour passer de pvalue a beta</t>
   </si>
+  <si>
+    <t>ICD10</t>
+  </si>
+  <si>
+    <t>C92</t>
+  </si>
 </sst>
 </file>
 
@@ -1135,7 +1141,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1223,6 +1229,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1504,10 +1513,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XEY91"/>
+  <dimension ref="A1:XEZ91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="C94" sqref="C94"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1515,18 +1524,19 @@
     <col min="1" max="1" width="22.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="11" style="2" customWidth="1"/>
     <col min="3" max="3" width="32.83203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="16.5" style="13" customWidth="1"/>
-    <col min="5" max="5" width="12" style="13" customWidth="1"/>
-    <col min="6" max="6" width="37.83203125" style="19" customWidth="1"/>
-    <col min="7" max="7" width="23.6640625" style="19" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" style="2" customWidth="1"/>
-    <col min="9" max="9" width="69" style="22" customWidth="1"/>
-    <col min="10" max="10" width="29.6640625" style="24" customWidth="1"/>
-    <col min="11" max="11" width="16.5" style="2" customWidth="1"/>
-    <col min="12" max="16384" width="10.83203125" style="2"/>
+    <col min="4" max="4" width="13.33203125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="16.5" style="13" customWidth="1"/>
+    <col min="6" max="6" width="12" style="13" customWidth="1"/>
+    <col min="7" max="7" width="37.83203125" style="19" customWidth="1"/>
+    <col min="8" max="8" width="23.6640625" style="19" customWidth="1"/>
+    <col min="9" max="9" width="20.83203125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="69" style="22" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="24" customWidth="1"/>
+    <col min="12" max="12" width="16.5" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1537,31 +1547,34 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="14" t="s">
+      <c r="G1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>215</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="2" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>42</v>
       </c>
@@ -1569,24 +1582,25 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="15"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="15"/>
-      <c r="H2" s="5"/>
+      <c r="H2" s="15"/>
       <c r="I2" s="5"/>
       <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
     </row>
-    <row r="3" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
         <v>83</v>
       </c>
       <c r="B3" s="8"/>
       <c r="C3" s="8"/>
-      <c r="D3" s="12"/>
+      <c r="D3" s="8"/>
       <c r="E3" s="12"/>
-      <c r="F3" s="16"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="16"/>
-      <c r="H3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="8"/>
       <c r="L3" s="8"/>
       <c r="M3" s="8"/>
       <c r="N3" s="8"/>
@@ -17955,8 +17969,9 @@
       <c r="XEW3" s="8"/>
       <c r="XEX3" s="8"/>
       <c r="XEY3" s="8"/>
+      <c r="XEZ3" s="8"/>
     </row>
-    <row r="4" spans="1:16379" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16380" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
         <v>1</v>
       </c>
@@ -17966,27 +17981,28 @@
       <c r="C4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="13">
+      <c r="D4" s="7"/>
+      <c r="E4" s="13">
         <v>322154</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="3">
+      <c r="H4" s="17"/>
+      <c r="I4" s="3">
         <v>84</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="J4" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J4" s="24" t="s">
+      <c r="K4" s="24" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="5" spans="1:16379" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16380" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
         <v>2</v>
       </c>
@@ -17994,27 +18010,28 @@
       <c r="C5" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="13">
+      <c r="D5" s="7"/>
+      <c r="E5" s="13">
         <v>210088</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="F5" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="3">
+      <c r="H5" s="17"/>
+      <c r="I5" s="3">
         <v>43</v>
       </c>
-      <c r="I5" s="24" t="s">
+      <c r="J5" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J5" s="24" t="s">
+      <c r="K5" s="24" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:16379" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16380" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9">
         <v>3</v>
       </c>
@@ -18024,27 +18041,28 @@
       <c r="C6" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="7"/>
+      <c r="E6" s="13">
         <v>188577</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="F6" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="3">
+      <c r="H6" s="17"/>
+      <c r="I6" s="3">
         <v>159</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="J6" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J6" s="24" t="s">
+      <c r="K6" s="24" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="7" spans="1:16379" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16380" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
         <v>4</v>
       </c>
@@ -18054,27 +18072,28 @@
       <c r="C7" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="13">
+      <c r="D7" s="7"/>
+      <c r="E7" s="13">
         <v>188577</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="F7" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G7" s="17"/>
-      <c r="H7" s="3">
+      <c r="H7" s="17"/>
+      <c r="I7" s="3">
         <v>141</v>
       </c>
-      <c r="I7" s="24" t="s">
+      <c r="J7" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="K7" s="24" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="8" spans="1:16379" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16380" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
         <v>5</v>
       </c>
@@ -18084,24 +18103,25 @@
       <c r="C8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D8" s="13">
+      <c r="D8" s="7"/>
+      <c r="E8" s="13">
         <v>188577</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="3">
+      <c r="H8" s="17"/>
+      <c r="I8" s="3">
         <v>101</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="J8" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="K8" s="24" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="9" spans="1:16379" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16380" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
         <v>6</v>
       </c>
@@ -18111,27 +18131,28 @@
       <c r="C9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="D9" s="13">
+      <c r="D9" s="7"/>
+      <c r="E9" s="13">
         <v>108039</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="F9" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="3">
+      <c r="H9" s="17"/>
+      <c r="I9" s="3">
         <v>29</v>
       </c>
-      <c r="I9" s="24" t="s">
+      <c r="J9" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J9" s="24" t="s">
+      <c r="K9" s="24" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="10" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
         <v>7</v>
       </c>
@@ -18141,27 +18162,28 @@
       <c r="C10" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D10" s="13">
+      <c r="D10" s="7"/>
+      <c r="E10" s="13">
         <v>108039</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="F10" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="17" t="s">
         <v>87</v>
       </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="3">
+      <c r="H10" s="17"/>
+      <c r="I10" s="3">
         <v>29</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="J10" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="K10" s="24" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="11" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9">
         <v>8</v>
       </c>
@@ -18171,27 +18193,28 @@
       <c r="C11" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="7"/>
+      <c r="E11" s="13">
         <v>253288</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="F11" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F11" s="17" t="s">
+      <c r="G11" s="17" t="s">
         <v>88</v>
       </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="3" t="s">
+      <c r="H11" s="17"/>
+      <c r="I11" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="I11" s="24" t="s">
+      <c r="J11" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J11" s="24" t="s">
+      <c r="K11" s="24" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="12" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -18201,38 +18224,40 @@
       <c r="C12" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="D12" s="13">
+      <c r="D12" s="7"/>
+      <c r="E12" s="13">
         <v>405072</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="F12" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="3" t="s">
+      <c r="H12" s="17"/>
+      <c r="I12" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="J12" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="K12" s="24" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="13" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3"/>
       <c r="B13" s="11"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="3"/>
+      <c r="D13" s="7"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="18"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="18"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="23"/>
+      <c r="H13" s="18"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="23"/>
     </row>
-    <row r="14" spans="1:16379" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16380" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>41</v>
       </c>
@@ -18240,19 +18265,20 @@
       <c r="C14" s="5"/>
       <c r="D14" s="5"/>
       <c r="E14" s="5"/>
-      <c r="F14" s="15"/>
+      <c r="F14" s="5"/>
       <c r="G14" s="15"/>
-      <c r="H14" s="5"/>
+      <c r="H14" s="15"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
+      <c r="K14" s="5"/>
     </row>
-    <row r="15" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="11"/>
     </row>
-    <row r="16" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
         <v>1</v>
       </c>
@@ -18262,24 +18288,24 @@
       <c r="C16" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="13">
+      <c r="E16" s="13">
         <v>108039</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="F16" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F16" s="20" t="s">
+      <c r="G16" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G16" s="20"/>
-      <c r="I16" s="24" t="s">
+      <c r="H16" s="20"/>
+      <c r="J16" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="K16" s="24" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
         <v>2</v>
       </c>
@@ -18287,24 +18313,24 @@
       <c r="C17" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="13">
+      <c r="E17" s="13">
         <v>108039</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="F17" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F17" s="20" t="s">
+      <c r="G17" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G17" s="20"/>
-      <c r="I17" s="24" t="s">
+      <c r="H17" s="20"/>
+      <c r="J17" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J17" s="24" t="s">
+      <c r="K17" s="24" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="9">
         <v>3</v>
       </c>
@@ -18312,24 +18338,24 @@
       <c r="C18" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="13">
+      <c r="E18" s="13">
         <v>108039</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="F18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="G18" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G18" s="20"/>
-      <c r="I18" s="24" t="s">
+      <c r="H18" s="20"/>
+      <c r="J18" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J18" s="24" t="s">
+      <c r="K18" s="24" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
         <v>4</v>
       </c>
@@ -18339,24 +18365,24 @@
       <c r="C19" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="13">
+      <c r="E19" s="13">
         <v>108039</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="G19" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G19" s="20"/>
-      <c r="I19" s="24" t="s">
+      <c r="H19" s="20"/>
+      <c r="J19" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="K19" s="24" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
         <v>5</v>
       </c>
@@ -18366,24 +18392,24 @@
       <c r="C20" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="13">
+      <c r="E20" s="13">
         <v>108039</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="F20" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="G20" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G20" s="20"/>
-      <c r="I20" s="24" t="s">
+      <c r="H20" s="20"/>
+      <c r="J20" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="K20" s="24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
         <v>6</v>
       </c>
@@ -18391,24 +18417,24 @@
       <c r="C21" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D21" s="13">
+      <c r="E21" s="13">
         <v>108039</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="F21" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="G21" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G21" s="20"/>
-      <c r="I21" s="24" t="s">
+      <c r="H21" s="20"/>
+      <c r="J21" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J21" s="24" t="s">
+      <c r="K21" s="24" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9">
         <v>7</v>
       </c>
@@ -18418,24 +18444,24 @@
       <c r="C22" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="13">
+      <c r="E22" s="13">
         <v>108039</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="F22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="G22" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G22" s="20"/>
-      <c r="I22" s="24" t="s">
+      <c r="H22" s="20"/>
+      <c r="J22" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J22" s="24" t="s">
+      <c r="K22" s="24" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
         <v>8</v>
       </c>
@@ -18445,24 +18471,24 @@
       <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="13">
+      <c r="E23" s="13">
         <v>108039</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="F23" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="G23" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G23" s="20"/>
-      <c r="I23" s="24" t="s">
+      <c r="H23" s="20"/>
+      <c r="J23" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J23" s="24" t="s">
+      <c r="K23" s="24" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
         <v>9</v>
       </c>
@@ -18470,24 +18496,24 @@
       <c r="C24" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="13">
+      <c r="E24" s="13">
         <v>108039</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="F24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="G24" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G24" s="20"/>
-      <c r="I24" s="24" t="s">
+      <c r="H24" s="20"/>
+      <c r="J24" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J24" s="24" t="s">
+      <c r="K24" s="24" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="9">
         <v>10</v>
       </c>
@@ -18495,24 +18521,24 @@
       <c r="C25" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D25" s="13">
+      <c r="E25" s="13">
         <v>108039</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="F25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="G25" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G25" s="20"/>
-      <c r="I25" s="24" t="s">
+      <c r="H25" s="20"/>
+      <c r="J25" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J25" s="24" t="s">
+      <c r="K25" s="24" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
         <v>11</v>
       </c>
@@ -18520,24 +18546,24 @@
       <c r="C26" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D26" s="13">
+      <c r="E26" s="13">
         <v>108039</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="F26" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="G26" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G26" s="20"/>
-      <c r="I26" s="24" t="s">
+      <c r="H26" s="20"/>
+      <c r="J26" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J26" s="24" t="s">
+      <c r="K26" s="24" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="9">
         <v>12</v>
       </c>
@@ -18545,24 +18571,24 @@
       <c r="C27" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D27" s="13">
+      <c r="E27" s="13">
         <v>108039</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="F27" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="G27" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G27" s="20"/>
-      <c r="I27" s="24" t="s">
+      <c r="H27" s="20"/>
+      <c r="J27" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J27" s="24" t="s">
+      <c r="K27" s="24" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="9">
         <v>13</v>
       </c>
@@ -18570,24 +18596,24 @@
       <c r="C28" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D28" s="13">
+      <c r="E28" s="13">
         <v>108039</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="F28" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="G28" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G28" s="20"/>
-      <c r="I28" s="24" t="s">
+      <c r="H28" s="20"/>
+      <c r="J28" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J28" s="24" t="s">
+      <c r="K28" s="24" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
         <v>14</v>
       </c>
@@ -18595,24 +18621,24 @@
       <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="13">
+      <c r="E29" s="13">
         <v>108039</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="F29" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="G29" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G29" s="20"/>
-      <c r="I29" s="24" t="s">
+      <c r="H29" s="20"/>
+      <c r="J29" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J29" s="24" t="s">
+      <c r="K29" s="24" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
         <v>15</v>
       </c>
@@ -18620,24 +18646,24 @@
       <c r="C30" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D30" s="13">
+      <c r="E30" s="13">
         <v>108039</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="F30" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="G30" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G30" s="20"/>
-      <c r="I30" s="24" t="s">
+      <c r="H30" s="20"/>
+      <c r="J30" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J30" s="24" t="s">
+      <c r="K30" s="24" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9">
         <v>16</v>
       </c>
@@ -18645,24 +18671,24 @@
       <c r="C31" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D31" s="13">
+      <c r="E31" s="13">
         <v>108039</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="F31" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="20" t="s">
+      <c r="G31" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G31" s="20"/>
-      <c r="I31" s="24" t="s">
+      <c r="H31" s="20"/>
+      <c r="J31" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J31" s="24" t="s">
+      <c r="K31" s="24" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
         <v>17</v>
       </c>
@@ -18672,24 +18698,24 @@
       <c r="C32" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="13">
+      <c r="E32" s="13">
         <v>108039</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="F32" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="20" t="s">
+      <c r="G32" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G32" s="20"/>
-      <c r="I32" s="24" t="s">
+      <c r="H32" s="20"/>
+      <c r="J32" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J32" s="24" t="s">
+      <c r="K32" s="24" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
         <v>18</v>
       </c>
@@ -18697,24 +18723,24 @@
       <c r="C33" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D33" s="13">
+      <c r="E33" s="13">
         <v>108039</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="F33" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="20" t="s">
+      <c r="G33" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G33" s="20"/>
-      <c r="I33" s="24" t="s">
+      <c r="H33" s="20"/>
+      <c r="J33" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J33" s="24" t="s">
+      <c r="K33" s="24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
         <v>19</v>
       </c>
@@ -18722,24 +18748,24 @@
       <c r="C34" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D34" s="13">
+      <c r="E34" s="13">
         <v>108039</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="F34" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="20" t="s">
+      <c r="G34" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G34" s="20"/>
-      <c r="I34" s="24" t="s">
+      <c r="H34" s="20"/>
+      <c r="J34" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J34" s="24" t="s">
+      <c r="K34" s="24" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9">
         <v>20</v>
       </c>
@@ -18749,24 +18775,24 @@
       <c r="C35" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="13">
+      <c r="E35" s="13">
         <v>108039</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="F35" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="G35" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G35" s="20"/>
-      <c r="I35" s="24" t="s">
+      <c r="H35" s="20"/>
+      <c r="J35" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J35" s="24" t="s">
+      <c r="K35" s="24" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
         <v>21</v>
       </c>
@@ -18774,24 +18800,24 @@
       <c r="C36" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D36" s="13">
+      <c r="E36" s="13">
         <v>108039</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="F36" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="G36" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="20"/>
-      <c r="I36" s="24" t="s">
+      <c r="H36" s="20"/>
+      <c r="J36" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J36" s="24" t="s">
+      <c r="K36" s="24" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
         <v>22</v>
       </c>
@@ -18799,24 +18825,24 @@
       <c r="C37" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D37" s="13">
+      <c r="E37" s="13">
         <v>108039</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="F37" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="G37" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G37" s="20"/>
-      <c r="I37" s="24" t="s">
+      <c r="H37" s="20"/>
+      <c r="J37" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J37" s="24" t="s">
+      <c r="K37" s="24" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
         <v>23</v>
       </c>
@@ -18826,33 +18852,33 @@
       <c r="C38" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D38" s="13">
+      <c r="E38" s="13">
         <v>108039</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="F38" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F38" s="20" t="s">
+      <c r="G38" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="G38" s="20"/>
-      <c r="I38" s="24" t="s">
+      <c r="H38" s="20"/>
+      <c r="J38" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J38" s="24" t="s">
+      <c r="K38" s="24" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B39" s="11"/>
     </row>
-    <row r="40" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="10" t="s">
         <v>51</v>
       </c>
       <c r="B40" s="11"/>
     </row>
-    <row r="41" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="9">
         <v>1</v>
       </c>
@@ -18862,21 +18888,21 @@
       <c r="C41" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D41" s="13" t="s">
+      <c r="E41" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="G41" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="G41" s="17"/>
-      <c r="I41" s="24" t="s">
+      <c r="H41" s="17"/>
+      <c r="J41" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J41" s="24" t="s">
+      <c r="K41" s="24" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="9">
         <v>2</v>
       </c>
@@ -18886,21 +18912,21 @@
       <c r="C42" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="13" t="s">
+      <c r="E42" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="F42" s="17" t="s">
+      <c r="G42" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="I42" s="24" t="s">
+      <c r="H42" s="17"/>
+      <c r="J42" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J42" s="24" t="s">
+      <c r="K42" s="24" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
         <v>3</v>
       </c>
@@ -18908,21 +18934,21 @@
       <c r="C43" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D43" s="13" t="s">
+      <c r="E43" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="G43" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="I43" s="24" t="s">
+      <c r="H43" s="17"/>
+      <c r="J43" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J43" s="24" t="s">
+      <c r="K43" s="24" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="9">
         <v>4</v>
       </c>
@@ -18930,21 +18956,21 @@
       <c r="C44" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D44" s="13" t="s">
+      <c r="E44" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="G44" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="G44" s="17"/>
-      <c r="I44" s="24" t="s">
+      <c r="H44" s="17"/>
+      <c r="J44" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J44" s="24" t="s">
+      <c r="K44" s="24" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="9">
         <v>5</v>
       </c>
@@ -18954,21 +18980,21 @@
       <c r="C45" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="13" t="s">
+      <c r="E45" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F45" s="17" t="s">
+      <c r="G45" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="G45" s="17"/>
-      <c r="I45" s="24" t="s">
+      <c r="H45" s="17"/>
+      <c r="J45" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J45" s="24" t="s">
+      <c r="K45" s="24" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="9">
         <v>6</v>
       </c>
@@ -18978,21 +19004,21 @@
       <c r="C46" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D46" s="13" t="s">
+      <c r="E46" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="G46" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="G46" s="17"/>
-      <c r="I46" s="24" t="s">
+      <c r="H46" s="17"/>
+      <c r="J46" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J46" s="24" t="s">
+      <c r="K46" s="24" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
         <v>7</v>
       </c>
@@ -19002,21 +19028,21 @@
       <c r="C47" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D47" s="13" t="s">
+      <c r="E47" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="G47" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="I47" s="24" t="s">
+      <c r="H47" s="17"/>
+      <c r="J47" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J47" s="24" t="s">
+      <c r="K47" s="24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
         <v>8</v>
       </c>
@@ -19026,21 +19052,21 @@
       <c r="C48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="E48" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="F48" s="17" t="s">
+      <c r="G48" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="G48" s="17"/>
-      <c r="I48" s="24" t="s">
+      <c r="H48" s="17"/>
+      <c r="J48" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J48" s="24" t="s">
+      <c r="K48" s="24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>9</v>
       </c>
@@ -19050,21 +19076,21 @@
       <c r="C49" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D49" s="13" t="s">
+      <c r="E49" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="F49" s="17" t="s">
+      <c r="G49" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="G49" s="17"/>
-      <c r="I49" s="24" t="s">
+      <c r="H49" s="17"/>
+      <c r="J49" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J49" s="24" t="s">
+      <c r="K49" s="24" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
         <v>10</v>
       </c>
@@ -19074,21 +19100,21 @@
       <c r="C50" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="E50" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="F50" s="17" t="s">
+      <c r="G50" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G50" s="17"/>
-      <c r="I50" s="24" t="s">
+      <c r="H50" s="17"/>
+      <c r="J50" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J50" s="24" t="s">
+      <c r="K50" s="24" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="51" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9">
         <v>11</v>
       </c>
@@ -19096,30 +19122,30 @@
       <c r="C51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D51" s="13" t="s">
+      <c r="E51" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="G51" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G51" s="17"/>
-      <c r="I51" s="24" t="s">
+      <c r="H51" s="17"/>
+      <c r="J51" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J51" s="24" t="s">
+      <c r="K51" s="24" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B52" s="11"/>
     </row>
-    <row r="53" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
         <v>217</v>
       </c>
       <c r="B53" s="11"/>
     </row>
-    <row r="54" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9">
         <v>1</v>
       </c>
@@ -19127,20 +19153,20 @@
       <c r="C54" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="G54" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I54" s="24" t="s">
+      <c r="J54" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J54" s="24" t="s">
+      <c r="K54" s="24" t="s">
         <v>154</v>
       </c>
-      <c r="K54" s="2" t="s">
+      <c r="L54" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
         <v>2</v>
       </c>
@@ -19148,20 +19174,20 @@
       <c r="C55" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="G55" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I55" s="24" t="s">
+      <c r="J55" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J55" s="24" t="s">
+      <c r="K55" s="24" t="s">
         <v>158</v>
       </c>
-      <c r="K55" s="2" t="s">
+      <c r="L55" s="2" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="56" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
         <v>3</v>
       </c>
@@ -19169,17 +19195,18 @@
       <c r="C56" s="26" t="s">
         <v>194</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="D56" s="26"/>
+      <c r="G56" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I56" s="24" t="s">
+      <c r="J56" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J56" s="24" t="s">
+      <c r="K56" s="24" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <v>4</v>
       </c>
@@ -19187,17 +19214,20 @@
       <c r="C57" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="D57" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="G57" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I57" s="24" t="s">
+      <c r="J57" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J57" s="24" t="s">
+      <c r="K57" s="24" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="58" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <v>5</v>
       </c>
@@ -19207,17 +19237,17 @@
       <c r="C58" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F58" s="31" t="s">
+      <c r="G58" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I58" s="24" t="s">
+      <c r="J58" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J58" s="24" t="s">
+      <c r="K58" s="24" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>6</v>
       </c>
@@ -19225,18 +19255,18 @@
       <c r="C59" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F59" s="31" t="s">
+      <c r="G59" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="G59" s="21"/>
-      <c r="I59" s="24" t="s">
+      <c r="H59" s="21"/>
+      <c r="J59" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J59" s="24" t="s">
+      <c r="K59" s="24" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>7</v>
       </c>
@@ -19244,17 +19274,17 @@
       <c r="C60" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="F60" s="31" t="s">
+      <c r="G60" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I60" s="24" t="s">
+      <c r="J60" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J60" s="24" t="s">
+      <c r="K60" s="24" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>8</v>
       </c>
@@ -19262,20 +19292,20 @@
       <c r="C61" s="2" t="s">
         <v>172</v>
       </c>
-      <c r="F61" s="31" t="s">
+      <c r="G61" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I61" s="24" t="s">
+      <c r="J61" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J61" s="24" t="s">
+      <c r="K61" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="K61" s="2" t="s">
+      <c r="L61" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="62" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>9</v>
       </c>
@@ -19285,20 +19315,20 @@
       <c r="C62" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="F62" s="31" t="s">
+      <c r="G62" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I62" s="24" t="s">
+      <c r="J62" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J62" s="24" t="s">
+      <c r="K62" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="K62" s="2" t="s">
+      <c r="L62" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="63" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
         <v>10</v>
       </c>
@@ -19308,17 +19338,17 @@
       <c r="C63" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F63" s="31" t="s">
+      <c r="G63" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I63" s="24" t="s">
+      <c r="J63" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J63" s="24" t="s">
+      <c r="K63" s="24" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="64" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9">
         <v>11</v>
       </c>
@@ -19326,20 +19356,20 @@
       <c r="C64" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="F64" s="31" t="s">
+      <c r="G64" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I64" s="24" t="s">
+      <c r="J64" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J64" s="24" t="s">
+      <c r="K64" s="24" t="s">
         <v>177</v>
       </c>
-      <c r="K64" s="2" t="s">
+      <c r="L64" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="65" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="9">
         <v>12</v>
       </c>
@@ -19349,17 +19379,17 @@
       <c r="C65" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F65" s="31" t="s">
+      <c r="G65" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I65" s="24" t="s">
+      <c r="J65" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J65" s="24" t="s">
+      <c r="K65" s="24" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="9">
         <v>13</v>
       </c>
@@ -19369,17 +19399,17 @@
       <c r="C66" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F66" s="31" t="s">
+      <c r="G66" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I66" s="24" t="s">
+      <c r="J66" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J66" s="24" t="s">
+      <c r="K66" s="24" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="67" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="9">
         <v>14</v>
       </c>
@@ -19387,17 +19417,17 @@
       <c r="C67" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="F67" s="31" t="s">
+      <c r="G67" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I67" s="24" t="s">
+      <c r="J67" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J67" s="24" t="s">
+      <c r="K67" s="24" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="68" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="9">
         <v>15</v>
       </c>
@@ -19407,17 +19437,17 @@
       <c r="C68" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="31" t="s">
+      <c r="G68" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I68" s="24" t="s">
+      <c r="J68" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J68" s="24" t="s">
+      <c r="K68" s="24" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="69" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="9">
         <v>16</v>
       </c>
@@ -19425,17 +19455,17 @@
       <c r="C69" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="F69" s="31" t="s">
+      <c r="G69" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I69" s="24" t="s">
+      <c r="J69" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J69" s="24" t="s">
+      <c r="K69" s="24" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="70" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="9">
         <v>17</v>
       </c>
@@ -19445,17 +19475,17 @@
       <c r="C70" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="F70" s="31" t="s">
+      <c r="G70" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I70" s="24" t="s">
+      <c r="J70" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J70" s="24" t="s">
+      <c r="K70" s="24" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="71" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="9">
         <v>18</v>
       </c>
@@ -19463,17 +19493,17 @@
       <c r="C71" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F71" s="31" t="s">
+      <c r="G71" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I71" s="24" t="s">
+      <c r="J71" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J71" s="24" t="s">
+      <c r="K71" s="24" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="72" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="9">
         <v>19</v>
       </c>
@@ -19481,20 +19511,20 @@
       <c r="C72" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="F72" s="31" t="s">
+      <c r="G72" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I72" s="24" t="s">
+      <c r="J72" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J72" s="24" t="s">
+      <c r="K72" s="24" t="s">
         <v>190</v>
       </c>
-      <c r="K72" s="2" t="s">
+      <c r="L72" s="2" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="73" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9">
         <v>20</v>
       </c>
@@ -19502,24 +19532,24 @@
       <c r="C73" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="F73" s="31" t="s">
+      <c r="G73" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="I73" s="24" t="s">
+      <c r="J73" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J73" s="24" t="s">
+      <c r="K73" s="24" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="75" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
         <v>218</v>
       </c>
       <c r="B75" s="11"/>
-      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
     </row>
-    <row r="76" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="9">
         <v>1</v>
       </c>
@@ -19529,17 +19559,17 @@
       <c r="C76" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F76" s="19" t="s">
+      <c r="G76" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I76" s="24" t="s">
+      <c r="J76" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J76" s="24" t="s">
+      <c r="K76" s="24" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="77" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="9">
         <v>2</v>
       </c>
@@ -19547,20 +19577,20 @@
       <c r="C77" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F77" s="19" t="s">
+      <c r="G77" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="I77" s="24" t="s">
+      <c r="J77" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J77" s="24" t="s">
+      <c r="K77" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="K77" s="2" t="s">
+      <c r="L77" s="2" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="78" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="9">
         <v>3</v>
       </c>
@@ -19568,17 +19598,17 @@
       <c r="C78" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="F78" s="19" t="s">
+      <c r="G78" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="I78" s="24" t="s">
+      <c r="J78" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J78" s="24" t="s">
+      <c r="K78" s="24" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="79" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="9">
         <v>4</v>
       </c>
@@ -19586,18 +19616,18 @@
       <c r="C79" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="F79" s="25" t="s">
+      <c r="G79" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="G79" s="25"/>
-      <c r="I79" s="24" t="s">
+      <c r="H79" s="25"/>
+      <c r="J79" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J79" s="24" t="s">
+      <c r="K79" s="24" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="80" spans="1:16379" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="9">
         <v>5</v>
       </c>
@@ -19607,23 +19637,23 @@
       <c r="C80" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="D80" s="35"/>
+      <c r="D80" s="34"/>
       <c r="E80" s="35"/>
-      <c r="F80" s="21" t="s">
+      <c r="F80" s="35"/>
+      <c r="G80" s="21" t="s">
         <v>106</v>
       </c>
-      <c r="G80" s="21"/>
-      <c r="H80" s="34"/>
-      <c r="I80" s="36" t="s">
+      <c r="H80" s="21"/>
+      <c r="I80" s="34"/>
+      <c r="J80" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="J80" s="36" t="s">
+      <c r="K80" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="K80" s="34" t="s">
+      <c r="L80" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="L80" s="34"/>
       <c r="M80" s="34"/>
       <c r="N80" s="34"/>
       <c r="O80" s="34"/>
@@ -35991,8 +36021,9 @@
       <c r="XEW80" s="34"/>
       <c r="XEX80" s="34"/>
       <c r="XEY80" s="34"/>
+      <c r="XEZ80" s="34"/>
     </row>
-    <row r="81" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9">
         <v>6</v>
       </c>
@@ -36000,26 +36031,26 @@
       <c r="C81" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="F81" s="19" t="s">
+      <c r="G81" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="I81" s="24" t="s">
+      <c r="J81" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J81" s="24" t="s">
+      <c r="K81" s="24" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="82" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B82" s="11"/>
     </row>
-    <row r="83" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="10" t="s">
         <v>97</v>
       </c>
       <c r="B83" s="11"/>
     </row>
-    <row r="84" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="9">
         <v>1</v>
       </c>
@@ -36029,27 +36060,27 @@
       <c r="C84" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="D84" s="13" t="s">
+      <c r="E84" s="13" t="s">
         <v>202</v>
       </c>
-      <c r="E84" s="13" t="s">
+      <c r="F84" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="F84" s="31" t="s">
+      <c r="G84" s="31" t="s">
         <v>200</v>
       </c>
-      <c r="G84" s="31"/>
-      <c r="I84" s="24" t="s">
+      <c r="H84" s="31"/>
+      <c r="J84" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J84" s="24" t="s">
+      <c r="K84" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="K84" s="2" t="s">
+      <c r="L84" s="2" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="85" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
         <v>2</v>
       </c>
@@ -36059,18 +36090,18 @@
       <c r="C85" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="E85" s="13" t="s">
         <v>205</v>
       </c>
-      <c r="F85" s="31" t="s">
+      <c r="G85" s="31" t="s">
         <v>203</v>
       </c>
-      <c r="G85" s="31"/>
-      <c r="I85" s="22" t="s">
+      <c r="H85" s="31"/>
+      <c r="J85" s="22" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="9">
         <v>4</v>
       </c>
@@ -36080,24 +36111,24 @@
       <c r="C86" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D86" s="13" t="s">
+      <c r="E86" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="F86" s="31" t="s">
+      <c r="G86" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="G86" s="31"/>
-      <c r="I86" s="24" t="s">
+      <c r="H86" s="31"/>
+      <c r="J86" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="J86" s="24" t="s">
+      <c r="K86" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="K86" s="2" t="s">
+      <c r="L86" s="2" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="87" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="9">
         <v>5</v>
       </c>
@@ -36107,18 +36138,18 @@
       <c r="C87" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="D87" s="32" t="s">
+      <c r="E87" s="32" t="s">
         <v>207</v>
       </c>
-      <c r="F87" s="31" t="s">
+      <c r="G87" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="G87" s="31"/>
-      <c r="I87" s="22" t="s">
+      <c r="H87" s="31"/>
+      <c r="J87" s="22" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="88" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="9">
         <v>6</v>
       </c>
@@ -36128,20 +36159,20 @@
       <c r="C88" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F88" s="19" t="s">
+      <c r="G88" s="19" t="s">
         <v>219</v>
       </c>
-      <c r="I88" s="24" t="s">
+      <c r="J88" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="J88" s="24" t="s">
+      <c r="K88" s="24" t="s">
         <v>220</v>
       </c>
-      <c r="K88" s="2" t="s">
+      <c r="L88" s="2" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="90" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="27" t="s">
         <v>196</v>
       </c>
@@ -36153,41 +36184,43 @@
         <f>COUNTIF(C4:C88, "*")</f>
         <v>74</v>
       </c>
+      <c r="D90" s="37"/>
     </row>
-    <row r="91" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C91" s="30">
         <f>C90-B90</f>
         <v>36</v>
       </c>
+      <c r="D91" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F16" r:id="rId1" display="Zhu et al. 2018"/>
-    <hyperlink ref="F17:F38" r:id="rId2" display="Zhu et al. 2018"/>
-    <hyperlink ref="F84" r:id="rId3"/>
-    <hyperlink ref="F85" r:id="rId4"/>
-    <hyperlink ref="F87" r:id="rId5"/>
-    <hyperlink ref="F86" r:id="rId6"/>
-    <hyperlink ref="F54" r:id="rId7"/>
-    <hyperlink ref="F55" r:id="rId8"/>
-    <hyperlink ref="F56" r:id="rId9"/>
-    <hyperlink ref="F57" r:id="rId10"/>
-    <hyperlink ref="F60" r:id="rId11"/>
-    <hyperlink ref="F63" r:id="rId12"/>
-    <hyperlink ref="F66" r:id="rId13"/>
-    <hyperlink ref="F69" r:id="rId14"/>
-    <hyperlink ref="F72" r:id="rId15"/>
-    <hyperlink ref="F58" r:id="rId16"/>
-    <hyperlink ref="F61" r:id="rId17"/>
-    <hyperlink ref="F64" r:id="rId18"/>
-    <hyperlink ref="F67" r:id="rId19"/>
-    <hyperlink ref="F70" r:id="rId20"/>
-    <hyperlink ref="F73" r:id="rId21"/>
-    <hyperlink ref="F59" r:id="rId22"/>
-    <hyperlink ref="F62" r:id="rId23"/>
-    <hyperlink ref="F65" r:id="rId24"/>
-    <hyperlink ref="F68" r:id="rId25"/>
-    <hyperlink ref="F71" r:id="rId26"/>
+    <hyperlink ref="G16" r:id="rId1" display="Zhu et al. 2018"/>
+    <hyperlink ref="G17:G38" r:id="rId2" display="Zhu et al. 2018"/>
+    <hyperlink ref="G84" r:id="rId3"/>
+    <hyperlink ref="G85" r:id="rId4"/>
+    <hyperlink ref="G87" r:id="rId5"/>
+    <hyperlink ref="G86" r:id="rId6"/>
+    <hyperlink ref="G54" r:id="rId7"/>
+    <hyperlink ref="G55" r:id="rId8"/>
+    <hyperlink ref="G56" r:id="rId9"/>
+    <hyperlink ref="G57" r:id="rId10"/>
+    <hyperlink ref="G60" r:id="rId11"/>
+    <hyperlink ref="G63" r:id="rId12"/>
+    <hyperlink ref="G66" r:id="rId13"/>
+    <hyperlink ref="G69" r:id="rId14"/>
+    <hyperlink ref="G72" r:id="rId15"/>
+    <hyperlink ref="G58" r:id="rId16"/>
+    <hyperlink ref="G61" r:id="rId17"/>
+    <hyperlink ref="G64" r:id="rId18"/>
+    <hyperlink ref="G67" r:id="rId19"/>
+    <hyperlink ref="G70" r:id="rId20"/>
+    <hyperlink ref="G73" r:id="rId21"/>
+    <hyperlink ref="G59" r:id="rId22"/>
+    <hyperlink ref="G62" r:id="rId23"/>
+    <hyperlink ref="G65" r:id="rId24"/>
+    <hyperlink ref="G68" r:id="rId25"/>
+    <hyperlink ref="G71" r:id="rId26"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
New GSMR with primary + secondary
</commit_message>
<xml_diff>
--- a/0_DATA/list_of_traits_GSMR.xlsx
+++ b/0_DATA/list_of_traits_GSMR.xlsx
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="list_of_traits_GSMR.csv" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="671" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="675" uniqueCount="292">
   <si>
     <t>Trait</t>
   </si>
@@ -939,9 +939,6 @@
     <t>/shares/compbio/Group-Wray/YanHoltz/DATA/GWAS/GWAS_SUMSTAT/</t>
   </si>
   <si>
-    <t>META_ANALYSIS_10K23_beta_se_correctGC1_pdgene_sharing_280317.tbl</t>
-  </si>
-  <si>
     <t>Better coming soon</t>
   </si>
   <si>
@@ -1000,6 +997,186 @@
   </si>
   <si>
     <t>Problem: How to go from Z score to Beta + Pvalue + standard error?</t>
+  </si>
+  <si>
+    <t>bmi_giant_2015.txt</t>
+  </si>
+  <si>
+    <t>Waist-to-hipratioadjustedforBMI</t>
+  </si>
+  <si>
+    <t>HDLcholesterol</t>
+  </si>
+  <si>
+    <t>LDLcholesterol</t>
+  </si>
+  <si>
+    <t>systolicbloodpressure</t>
+  </si>
+  <si>
+    <t>diastolicbloodpressure</t>
+  </si>
+  <si>
+    <t>EduYear</t>
+  </si>
+  <si>
+    <t>allergicrhinitis</t>
+  </si>
+  <si>
+    <t>cardiovasculardisease</t>
+  </si>
+  <si>
+    <t>majordepressivedisorder</t>
+  </si>
+  <si>
+    <t>typeIIdiabetes</t>
+  </si>
+  <si>
+    <t>combined_ukb_gera_DIA2_1000g_m01_u05_geno.txt</t>
+  </si>
+  <si>
+    <t>hypertensivedisease</t>
+  </si>
+  <si>
+    <t>herniaabdominopelviccavity</t>
+  </si>
+  <si>
+    <t>irondeficiencyanemias</t>
+  </si>
+  <si>
+    <t>irritablebowelsyndrome</t>
+  </si>
+  <si>
+    <t>maculardegeneration</t>
+  </si>
+  <si>
+    <t>combined_ukb_gera_OSTIOA_1000g_m01_u05_geno.txt</t>
+  </si>
+  <si>
+    <t>combined_ukb_gera_OSTIOP_1000g_m01_u05_geno.txt</t>
+  </si>
+  <si>
+    <t>peripheralvasculardisease</t>
+  </si>
+  <si>
+    <t>combined_ukb_gera_PVD_1000g_m01_u05_geno.txt</t>
+  </si>
+  <si>
+    <t>pepticulcers</t>
+  </si>
+  <si>
+    <t>combined_ukb_gera_PEPTIC_ULCERS_1000g_m01_u05_geno.txt</t>
+  </si>
+  <si>
+    <t>psychiatricdisorder</t>
+  </si>
+  <si>
+    <t>acutereactiontostress</t>
+  </si>
+  <si>
+    <t>combined_ukb_gera_STRESS_1000g_m01_u05_geno.txt</t>
+  </si>
+  <si>
+    <t>varicoseveinsoflowerextremities</t>
+  </si>
+  <si>
+    <t>diseasecount</t>
+  </si>
+  <si>
+    <t>cad_cardiogram_2015.txt</t>
+  </si>
+  <si>
+    <t>RheumatoidArthritis</t>
+  </si>
+  <si>
+    <t>Crohn'sDisease</t>
+  </si>
+  <si>
+    <t>UlcerativeColitis</t>
+  </si>
+  <si>
+    <t>AutismSpectrumDisorder</t>
+  </si>
+  <si>
+    <t>BipolarDisorder</t>
+  </si>
+  <si>
+    <t>MajorDepressiveDisorder</t>
+  </si>
+  <si>
+    <t>Alzheimer'sDisease</t>
+  </si>
+  <si>
+    <t>AgedMacularDegeneration</t>
+  </si>
+  <si>
+    <t>Basophilcount</t>
+  </si>
+  <si>
+    <t>baso_cam_2016.txt</t>
+  </si>
+  <si>
+    <t>Eosinophilicesophagitis</t>
+  </si>
+  <si>
+    <t>Granulocytecount</t>
+  </si>
+  <si>
+    <t>ImmatureFractionofReticulocytes</t>
+  </si>
+  <si>
+    <t>Lymphocytecount</t>
+  </si>
+  <si>
+    <t>MeanCorpuscularHemoglobin</t>
+  </si>
+  <si>
+    <t>Meancorpuscularvolume</t>
+  </si>
+  <si>
+    <t>Monocytecount</t>
+  </si>
+  <si>
+    <t>Meanplateletvolume</t>
+  </si>
+  <si>
+    <t>Neutrophil(x4)</t>
+  </si>
+  <si>
+    <t>Plateletditributionwidth</t>
+  </si>
+  <si>
+    <t>PlateletCount</t>
+  </si>
+  <si>
+    <t>Redbloodcellcount</t>
+  </si>
+  <si>
+    <t>Redcelldistributionwidth</t>
+  </si>
+  <si>
+    <t>Reticulocytecount</t>
+  </si>
+  <si>
+    <t>Whitebloodcellcount</t>
+  </si>
+  <si>
+    <t>DepressiveSymptoms</t>
+  </si>
+  <si>
+    <t>IQ(UKB)</t>
+  </si>
+  <si>
+    <t>Wellbeing(x2)</t>
+  </si>
+  <si>
+    <t>Dementia-Alzheimer</t>
+  </si>
+  <si>
+    <t>META_ANALYSIS_10K23_beta_se_correctGC1_pdgene_sharing_280317.ma</t>
+  </si>
+  <si>
+    <t>Parkinson</t>
   </si>
 </sst>
 </file>
@@ -1547,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XEZ98"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="J86" sqref="J86:K86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1579,7 +1756,7 @@
         <v>0</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>1</v>
@@ -1591,7 +1768,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>49</v>
@@ -18607,7 +18784,7 @@
         <v>26</v>
       </c>
       <c r="D27" s="39" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E27" s="13">
         <v>108039</v>
@@ -18635,7 +18812,7 @@
         <v>27</v>
       </c>
       <c r="D28" s="39" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E28" s="13">
         <v>108039</v>
@@ -19051,7 +19228,7 @@
         <v>56</v>
       </c>
       <c r="D46" s="13" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E46" s="13" t="s">
         <v>75</v>
@@ -19190,7 +19367,7 @@
     </row>
     <row r="53" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="10" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B53" s="11"/>
     </row>
@@ -19299,7 +19476,7 @@
       </c>
       <c r="B59" s="11"/>
       <c r="C59" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="G59" s="31" t="s">
         <v>102</v>
@@ -19590,7 +19767,7 @@
     </row>
     <row r="75" spans="1:16380" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="10" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B75" s="11"/>
       <c r="J75" s="24"/>
@@ -36107,7 +36284,7 @@
         <v>199</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E84" s="13" t="s">
         <v>202</v>
@@ -36123,7 +36300,7 @@
         <v>108</v>
       </c>
       <c r="K84" s="24" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="L84" s="2" t="s">
         <v>201</v>
@@ -36171,10 +36348,10 @@
         <v>211</v>
       </c>
       <c r="K86" s="24" t="s">
+        <v>290</v>
+      </c>
+      <c r="L86" s="2" t="s">
         <v>212</v>
-      </c>
-      <c r="L86" s="2" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="87" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -36209,16 +36386,16 @@
         <v>101</v>
       </c>
       <c r="G88" s="19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J88" s="24" t="s">
         <v>108</v>
       </c>
       <c r="K88" s="24" t="s">
+        <v>219</v>
+      </c>
+      <c r="L88" s="2" t="s">
         <v>220</v>
-      </c>
-      <c r="L88" s="2" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -36244,7 +36421,7 @@
     </row>
     <row r="94" spans="1:12" s="4" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
@@ -36259,7 +36436,7 @@
     </row>
     <row r="95" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="96" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -36267,13 +36444,13 @@
         <v>1</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="G96" s="19" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J96" s="24" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="97" spans="1:3" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -36284,7 +36461,7 @@
     <row r="98" spans="1:3" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="9"/>
       <c r="C98" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>
@@ -36322,10 +36499,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -36362,12 +36539,12 @@
         <v>108</v>
       </c>
       <c r="D2" s="26" t="s">
-        <v>133</v>
+        <v>232</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="26" t="s">
-        <v>43</v>
+        <v>233</v>
       </c>
       <c r="C3" s="26" t="s">
         <v>108</v>
@@ -36381,7 +36558,7 @@
         <v>96</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>44</v>
+        <v>234</v>
       </c>
       <c r="C4" s="26" t="s">
         <v>108</v>
@@ -36395,7 +36572,7 @@
         <v>96</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>45</v>
+        <v>235</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>108</v>
@@ -36423,7 +36600,7 @@
         <v>96</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>47</v>
+        <v>236</v>
       </c>
       <c r="C7" s="26" t="s">
         <v>108</v>
@@ -36437,7 +36614,7 @@
         <v>96</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>48</v>
+        <v>237</v>
       </c>
       <c r="C8" s="26" t="s">
         <v>108</v>
@@ -36465,7 +36642,7 @@
         <v>96</v>
       </c>
       <c r="B10" s="26" t="s">
-        <v>84</v>
+        <v>238</v>
       </c>
       <c r="C10" s="26" t="s">
         <v>108</v>
@@ -36490,7 +36667,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="26" t="s">
-        <v>17</v>
+        <v>239</v>
       </c>
       <c r="C12" s="26" t="s">
         <v>108</v>
@@ -36501,7 +36678,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="26" t="s">
-        <v>18</v>
+        <v>240</v>
       </c>
       <c r="C13" s="26" t="s">
         <v>108</v>
@@ -36529,7 +36706,7 @@
         <v>96</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>92</v>
+        <v>241</v>
       </c>
       <c r="C15" s="26" t="s">
         <v>108</v>
@@ -36554,13 +36731,13 @@
         <v>96</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="C17" s="26" t="s">
         <v>108</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>116</v>
+        <v>243</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -36579,7 +36756,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="26" t="s">
-        <v>23</v>
+        <v>244</v>
       </c>
       <c r="C19" s="26" t="s">
         <v>108</v>
@@ -36601,7 +36778,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="26" t="s">
-        <v>25</v>
+        <v>245</v>
       </c>
       <c r="C21" s="26" t="s">
         <v>108</v>
@@ -36623,7 +36800,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="26" t="s">
-        <v>27</v>
+        <v>246</v>
       </c>
       <c r="C23" s="26" t="s">
         <v>108</v>
@@ -36634,7 +36811,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="26" t="s">
-        <v>28</v>
+        <v>247</v>
       </c>
       <c r="C24" s="26" t="s">
         <v>108</v>
@@ -36645,7 +36822,7 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B25" s="26" t="s">
-        <v>29</v>
+        <v>248</v>
       </c>
       <c r="C25" s="26" t="s">
         <v>108</v>
@@ -36662,7 +36839,7 @@
         <v>108</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>125</v>
+        <v>249</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -36676,29 +36853,29 @@
         <v>108</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>126</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="26" t="s">
-        <v>32</v>
+        <v>251</v>
       </c>
       <c r="C28" s="26" t="s">
         <v>108</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>129</v>
+        <v>252</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="26" t="s">
-        <v>33</v>
+        <v>253</v>
       </c>
       <c r="C29" s="26" t="s">
         <v>108</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>127</v>
+        <v>254</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -36706,7 +36883,7 @@
         <v>96</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>34</v>
+        <v>255</v>
       </c>
       <c r="C30" s="26" t="s">
         <v>108</v>
@@ -36717,18 +36894,18 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="26" t="s">
-        <v>35</v>
+        <v>256</v>
       </c>
       <c r="C31" s="26" t="s">
         <v>108</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>130</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="26" t="s">
-        <v>36</v>
+        <v>258</v>
       </c>
       <c r="C32" s="26" t="s">
         <v>108</v>
@@ -36742,7 +36919,7 @@
         <v>96</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>37</v>
+        <v>259</v>
       </c>
       <c r="C33" s="26" t="s">
         <v>108</v>
@@ -36762,7 +36939,7 @@
         <v>108</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>143</v>
+        <v>260</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -36770,7 +36947,7 @@
         <v>96</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>53</v>
+        <v>261</v>
       </c>
       <c r="C35" s="26" t="s">
         <v>108</v>
@@ -36781,7 +36958,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="26" t="s">
-        <v>54</v>
+        <v>262</v>
       </c>
       <c r="C36" s="26" t="s">
         <v>108</v>
@@ -36792,7 +36969,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="26" t="s">
-        <v>55</v>
+        <v>263</v>
       </c>
       <c r="C37" s="26" t="s">
         <v>108</v>
@@ -36806,7 +36983,7 @@
         <v>96</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="C38" s="26" t="s">
         <v>108</v>
@@ -36820,7 +36997,7 @@
         <v>96</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>56</v>
+        <v>264</v>
       </c>
       <c r="C39" s="26" t="s">
         <v>108</v>
@@ -36834,7 +37011,7 @@
         <v>96</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>57</v>
+        <v>265</v>
       </c>
       <c r="C40" s="26" t="s">
         <v>108</v>
@@ -36848,7 +37025,7 @@
         <v>96</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>58</v>
+        <v>266</v>
       </c>
       <c r="C41" s="26" t="s">
         <v>108</v>
@@ -36876,7 +37053,7 @@
         <v>96</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>59</v>
+        <v>267</v>
       </c>
       <c r="C43" s="26" t="s">
         <v>108</v>
@@ -36887,7 +37064,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B44" s="26" t="s">
-        <v>4</v>
+        <v>268</v>
       </c>
       <c r="C44" s="26" t="s">
         <v>108</v>
@@ -36898,18 +37075,18 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="26" t="s">
-        <v>197</v>
+        <v>269</v>
       </c>
       <c r="C45" s="26" t="s">
         <v>108</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>154</v>
+        <v>270</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B46" s="26" t="s">
-        <v>159</v>
+        <v>271</v>
       </c>
       <c r="C46" s="26" t="s">
         <v>108</v>
@@ -36920,7 +37097,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="26" t="s">
-        <v>194</v>
+        <v>272</v>
       </c>
       <c r="C47" s="26" t="s">
         <v>108</v>
@@ -36956,7 +37133,7 @@
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B50" s="26" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C50" s="26" t="s">
         <v>108</v>
@@ -36967,7 +37144,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B51" s="26" t="s">
-        <v>169</v>
+        <v>273</v>
       </c>
       <c r="C51" s="26" t="s">
         <v>108</v>
@@ -36978,7 +37155,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" s="26" t="s">
-        <v>172</v>
+        <v>274</v>
       </c>
       <c r="C52" s="26" t="s">
         <v>108</v>
@@ -36992,7 +37169,7 @@
         <v>96</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>174</v>
+        <v>275</v>
       </c>
       <c r="C53" s="26" t="s">
         <v>108</v>
@@ -37006,7 +37183,7 @@
         <v>96</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>10</v>
+        <v>276</v>
       </c>
       <c r="C54" s="26" t="s">
         <v>108</v>
@@ -37017,7 +37194,7 @@
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B55" s="26" t="s">
-        <v>176</v>
+        <v>277</v>
       </c>
       <c r="C55" s="26" t="s">
         <v>108</v>
@@ -37031,7 +37208,7 @@
         <v>96</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>11</v>
+        <v>278</v>
       </c>
       <c r="C56" s="26" t="s">
         <v>108</v>
@@ -37045,7 +37222,7 @@
         <v>96</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>93</v>
+        <v>279</v>
       </c>
       <c r="C57" s="26" t="s">
         <v>108</v>
@@ -37070,7 +37247,7 @@
         <v>96</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>13</v>
+        <v>280</v>
       </c>
       <c r="C59" s="26" t="s">
         <v>108</v>
@@ -37081,7 +37258,7 @@
     </row>
     <row r="60" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B60" s="26" t="s">
-        <v>184</v>
+        <v>281</v>
       </c>
       <c r="C60" s="26" t="s">
         <v>108</v>
@@ -37095,7 +37272,7 @@
         <v>96</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>186</v>
+        <v>282</v>
       </c>
       <c r="C61" s="26" t="s">
         <v>108</v>
@@ -37106,7 +37283,7 @@
     </row>
     <row r="62" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="26" t="s">
-        <v>14</v>
+        <v>283</v>
       </c>
       <c r="C62" s="26" t="s">
         <v>108</v>
@@ -37117,7 +37294,7 @@
     </row>
     <row r="63" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B63" s="26" t="s">
-        <v>189</v>
+        <v>284</v>
       </c>
       <c r="C63" s="26" t="s">
         <v>108</v>
@@ -37128,7 +37305,7 @@
     </row>
     <row r="64" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B64" s="26" t="s">
-        <v>191</v>
+        <v>285</v>
       </c>
       <c r="C64" s="26" t="s">
         <v>108</v>
@@ -37142,7 +37319,7 @@
         <v>96</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>6</v>
+        <v>286</v>
       </c>
       <c r="C65" s="26" t="s">
         <v>108</v>
@@ -37175,7 +37352,7 @@
     </row>
     <row r="68" spans="1:4" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="26" t="s">
-        <v>103</v>
+        <v>287</v>
       </c>
       <c r="C68" s="26" t="s">
         <v>108</v>
@@ -37200,7 +37377,7 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B70" s="26" t="s">
-        <v>94</v>
+        <v>288</v>
       </c>
       <c r="C70" s="26" t="s">
         <v>108</v>
@@ -37214,13 +37391,27 @@
         <v>96</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>199</v>
+        <v>289</v>
       </c>
       <c r="C71" s="26" t="s">
         <v>108</v>
       </c>
       <c r="D71" s="26" t="s">
-        <v>214</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A72" s="26" t="s">
+        <v>96</v>
+      </c>
+      <c r="B72" s="26" t="s">
+        <v>291</v>
+      </c>
+      <c r="C72" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="D72" s="26" t="s">
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Schizophrenia was missing in GSMR
</commit_message>
<xml_diff>
--- a/0_DATA/list_of_traits_GSMR.xlsx
+++ b/0_DATA/list_of_traits_GSMR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="37780" windowHeight="19480" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="-38160" yWindow="460" windowWidth="37780" windowHeight="19480" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1724,8 +1724,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XEZ98"/>
   <sheetViews>
-    <sheetView topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="J86" sqref="J86:K86"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -18310,7 +18310,7 @@
         <v>96</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D8" s="7"/>
       <c r="E8" s="13">
@@ -36453,16 +36453,28 @@
         <v>228</v>
       </c>
     </row>
-    <row r="97" spans="1:3" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="9">
         <v>642</v>
       </c>
+      <c r="E97" s="2"/>
+      <c r="F97" s="2"/>
+      <c r="G97" s="2"/>
+      <c r="H97" s="2"/>
+      <c r="J97" s="2"/>
+      <c r="K97" s="2"/>
     </row>
-    <row r="98" spans="1:3" s="2" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:11" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="9"/>
       <c r="C98" s="2" t="s">
         <v>231</v>
       </c>
+      <c r="E98" s="2"/>
+      <c r="F98" s="2"/>
+      <c r="G98" s="2"/>
+      <c r="H98" s="2"/>
+      <c r="J98" s="2"/>
+      <c r="K98" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -36501,8 +36513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
MtCOJO smoke + BMI OK
</commit_message>
<xml_diff>
--- a/0_DATA/list_of_traits_GSMR.xlsx
+++ b/0_DATA/list_of_traits_GSMR.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="297">
   <si>
     <t>Trait</t>
   </si>
@@ -1151,6 +1151,27 @@
   <si>
     <t>Need to be published first</t>
   </si>
+  <si>
+    <t>Outdoor activity</t>
+  </si>
+  <si>
+    <t>Smoking</t>
+  </si>
+  <si>
+    <t>Burning on UV exposure</t>
+  </si>
+  <si>
+    <t>Dark skin</t>
+  </si>
+  <si>
+    <t>Gerstenblith et al. Used by Bonilla et al.</t>
+  </si>
+  <si>
+    <t>Angli, in press</t>
+  </si>
+  <si>
+    <t>ukbEUR_SI_cojo.txt</t>
+  </si>
 </sst>
 </file>
 
@@ -1697,7 +1718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XEZ101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
       <selection activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
@@ -36350,21 +36371,50 @@
     <row r="88" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="9"/>
       <c r="B88" s="11"/>
-      <c r="J88" s="24"/>
+      <c r="C88" s="2" t="s">
+        <v>291</v>
+      </c>
+      <c r="F88" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G88" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="J88" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="K88" s="24" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="89" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9"/>
       <c r="B89" s="11"/>
+      <c r="C89" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="J89" s="24"/>
     </row>
     <row r="90" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="9"/>
       <c r="B90" s="11"/>
+      <c r="C90" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G90" s="31" t="s">
+        <v>294</v>
+      </c>
       <c r="J90" s="24"/>
     </row>
     <row r="91" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="9"/>
       <c r="B91" s="11"/>
+      <c r="C91" s="2" t="s">
+        <v>293</v>
+      </c>
+      <c r="G91" s="31" t="s">
+        <v>294</v>
+      </c>
       <c r="J91" s="24"/>
     </row>
     <row r="93" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
@@ -36473,6 +36523,8 @@
     <hyperlink ref="G64" r:id="rId24"/>
     <hyperlink ref="G67" r:id="rId25"/>
     <hyperlink ref="G70" r:id="rId26"/>
+    <hyperlink ref="G90" r:id="rId27"/>
+    <hyperlink ref="G91" r:id="rId28"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
First version of integrated plot
</commit_message>
<xml_diff>
--- a/0_DATA/list_of_traits_GSMR.xlsx
+++ b/0_DATA/list_of_traits_GSMR.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38160" yWindow="460" windowWidth="37780" windowHeight="19480" tabRatio="500"/>
+    <workbookView xWindow="-38160" yWindow="460" windowWidth="38160" windowHeight="20940" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="683" uniqueCount="298">
   <si>
     <t>Trait</t>
   </si>
@@ -1152,9 +1152,6 @@
     <t>Need to be published first</t>
   </si>
   <si>
-    <t>Outdoor activity</t>
-  </si>
-  <si>
     <t>Smoking</t>
   </si>
   <si>
@@ -1171,6 +1168,12 @@
   </si>
   <si>
     <t>ukbEUR_SI_cojo.txt</t>
+  </si>
+  <si>
+    <t>Outdoor activity IPAQ</t>
+  </si>
+  <si>
+    <t>ukbEUR_MAF1e-4_IPAQG.bolt.ma</t>
   </si>
 </sst>
 </file>
@@ -1719,7 +1722,7 @@
   <dimension ref="A1:XEZ101"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
-      <selection activeCell="J90" sqref="J90"/>
+      <selection activeCell="G95" sqref="G95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="17" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -36372,37 +36375,54 @@
       <c r="A88" s="9"/>
       <c r="B88" s="11"/>
       <c r="C88" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
+      </c>
+      <c r="E88" s="13">
+        <v>456426</v>
       </c>
       <c r="F88" s="13" t="s">
         <v>38</v>
       </c>
       <c r="G88" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="J88" s="24" t="s">
         <v>106</v>
       </c>
       <c r="K88" s="24" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9"/>
       <c r="B89" s="11"/>
       <c r="C89" s="2" t="s">
-        <v>290</v>
-      </c>
-      <c r="J89" s="24"/>
+        <v>296</v>
+      </c>
+      <c r="E89" s="13">
+        <v>456426</v>
+      </c>
+      <c r="F89" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="G89" s="19" t="s">
+        <v>294</v>
+      </c>
+      <c r="J89" s="24" t="s">
+        <v>106</v>
+      </c>
+      <c r="K89" s="24" t="s">
+        <v>297</v>
+      </c>
     </row>
     <row r="90" spans="1:12" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="9"/>
       <c r="B90" s="11"/>
       <c r="C90" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G90" s="31" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="J90" s="24"/>
     </row>
@@ -36410,10 +36430,10 @@
       <c r="A91" s="9"/>
       <c r="B91" s="11"/>
       <c r="C91" s="2" t="s">
+        <v>292</v>
+      </c>
+      <c r="G91" s="31" t="s">
         <v>293</v>
-      </c>
-      <c r="G91" s="31" t="s">
-        <v>294</v>
       </c>
       <c r="J91" s="24"/>
     </row>

</xml_diff>